<commit_message>
Add outputs (tables, charts, summaries) for CTDC analysis
</commit_message>
<xml_diff>
--- a/outputs/missing_summary_styled.xlsx
+++ b/outputs/missing_summary_styled.xlsx
@@ -35,7 +35,7 @@
       <color rgb="00000000"/>
     </font>
   </fonts>
-  <fills count="41">
+  <fills count="80">
     <fill>
       <patternFill/>
     </fill>
@@ -235,6 +235,201 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="00FFF5F0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0008306B"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0008316D"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00083573"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00083979"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00083B7C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00083C7D"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00083D7F"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00084488"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0008458A"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0008468B"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00084B93"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00084C95"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00084E98"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0008509B"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0008519C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="000A539E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="001460A8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="002676B8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="002A7AB9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="002B7BBA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="004493C7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="006CAED6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0077B5D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="008ABFDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="008CC0DD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0091C3DE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="009AC8E0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="009CC9E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="009FCAE1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00A1CBE2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00A3CCE3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00A9CFE5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00ABD0E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00BDD7EC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00C4DAEE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00DAE8F6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E7F0FA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F4F9FE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F7FBFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -256,50 +451,89 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="41" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="42" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="43" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="44" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="45" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="46" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="47" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="48" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="49" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="50" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="51" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="52" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="53" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="54" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="16" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="55" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="17" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="56" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="18" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="57" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="19" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="58" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="59" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="21" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="60" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="22" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="61" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="23" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="62" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="24" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="63" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="25" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="64" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="26" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="65" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="27" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="66" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="28" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="67" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="29" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="68" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="30" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="69" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="31" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="70" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="32" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="71" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="33" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="72" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="34" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="73" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="35" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="74" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="36" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="75" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="37" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="76" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="38" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="77" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="39" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="78" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="40" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="79" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -699,7 +933,7 @@
       <c r="B2" s="2" t="n">
         <v>93841</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2" s="3" t="n">
         <v>96</v>
       </c>
     </row>
@@ -709,10 +943,10 @@
           <t>meansOfControlRestrictsFinancialAccess</t>
         </is>
       </c>
-      <c r="B3" s="3" t="n">
+      <c r="B3" s="4" t="n">
         <v>93419</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3" s="5" t="n">
         <v>95.56999999999999</v>
       </c>
     </row>
@@ -722,10 +956,10 @@
           <t>meansOfControlRestrictsMedicalCare</t>
         </is>
       </c>
-      <c r="B4" s="4" t="n">
+      <c r="B4" s="6" t="n">
         <v>91779</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4" s="7" t="n">
         <v>93.89</v>
       </c>
     </row>
@@ -735,10 +969,10 @@
           <t>majorityEntry</t>
         </is>
       </c>
-      <c r="B5" s="5" t="n">
+      <c r="B5" s="8" t="n">
         <v>90498</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5" s="9" t="n">
         <v>92.58</v>
       </c>
     </row>
@@ -748,10 +982,10 @@
           <t>meansOfControlFalsePromises</t>
         </is>
       </c>
-      <c r="B6" s="6" t="n">
+      <c r="B6" s="10" t="n">
         <v>89626</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6" s="11" t="n">
         <v>91.69</v>
       </c>
     </row>
@@ -761,10 +995,10 @@
           <t>meansOfControlDebtBondage</t>
         </is>
       </c>
-      <c r="B7" s="6" t="n">
+      <c r="B7" s="10" t="n">
         <v>89515</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C7" s="11" t="n">
         <v>91.58</v>
       </c>
     </row>
@@ -774,10 +1008,10 @@
           <t>meansOfControlWithholdsDocuments</t>
         </is>
       </c>
-      <c r="B8" s="6" t="n">
+      <c r="B8" s="10" t="n">
         <v>89466</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C8" s="11" t="n">
         <v>91.53</v>
       </c>
     </row>
@@ -787,10 +1021,10 @@
           <t>meansOfControlExcessiveWorkingHours</t>
         </is>
       </c>
-      <c r="B9" s="7" t="n">
+      <c r="B9" s="12" t="n">
         <v>89121</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C9" s="13" t="n">
         <v>91.17</v>
       </c>
     </row>
@@ -800,10 +1034,10 @@
           <t>isSlaveryAndPractices</t>
         </is>
       </c>
-      <c r="B10" s="8" t="n">
+      <c r="B10" s="14" t="n">
         <v>88874</v>
       </c>
-      <c r="C10" t="n">
+      <c r="C10" s="15" t="n">
         <v>90.92</v>
       </c>
     </row>
@@ -813,10 +1047,10 @@
           <t>meansOfControlWithholdsNecessities</t>
         </is>
       </c>
-      <c r="B11" s="8" t="n">
+      <c r="B11" s="14" t="n">
         <v>88864</v>
       </c>
-      <c r="C11" t="n">
+      <c r="C11" s="15" t="n">
         <v>90.91</v>
       </c>
     </row>
@@ -826,10 +1060,10 @@
           <t>meansOfControlThreatOfLawEnforcement</t>
         </is>
       </c>
-      <c r="B12" s="8" t="n">
+      <c r="B12" s="14" t="n">
         <v>88827</v>
       </c>
-      <c r="C12" t="n">
+      <c r="C12" s="15" t="n">
         <v>90.87</v>
       </c>
     </row>
@@ -839,10 +1073,10 @@
           <t>meansOfControlSexualAbuse</t>
         </is>
       </c>
-      <c r="B13" s="8" t="n">
+      <c r="B13" s="14" t="n">
         <v>88737</v>
       </c>
-      <c r="C13" t="n">
+      <c r="C13" s="15" t="n">
         <v>90.78</v>
       </c>
     </row>
@@ -852,10 +1086,10 @@
           <t>meansOfControlPsychoactiveSubstances</t>
         </is>
       </c>
-      <c r="B14" s="9" t="n">
+      <c r="B14" s="16" t="n">
         <v>86778</v>
       </c>
-      <c r="C14" t="n">
+      <c r="C14" s="17" t="n">
         <v>88.78</v>
       </c>
     </row>
@@ -865,10 +1099,10 @@
           <t>meansOfControlTakesEarnings</t>
         </is>
       </c>
-      <c r="B15" s="10" t="n">
+      <c r="B15" s="18" t="n">
         <v>86312</v>
       </c>
-      <c r="C15" t="n">
+      <c r="C15" s="19" t="n">
         <v>88.3</v>
       </c>
     </row>
@@ -878,10 +1112,10 @@
           <t>meansOfControlOther</t>
         </is>
       </c>
-      <c r="B16" s="11" t="n">
+      <c r="B16" s="20" t="n">
         <v>86146</v>
       </c>
-      <c r="C16" t="n">
+      <c r="C16" s="21" t="n">
         <v>88.13</v>
       </c>
     </row>
@@ -891,10 +1125,10 @@
           <t>meansOfControlPhysicalAbuse</t>
         </is>
       </c>
-      <c r="B17" s="11" t="n">
+      <c r="B17" s="20" t="n">
         <v>85817</v>
       </c>
-      <c r="C17" t="n">
+      <c r="C17" s="21" t="n">
         <v>87.79000000000001</v>
       </c>
     </row>
@@ -904,10 +1138,10 @@
           <t>isForcedMarriage</t>
         </is>
       </c>
-      <c r="B18" s="12" t="n">
+      <c r="B18" s="22" t="n">
         <v>84246</v>
       </c>
-      <c r="C18" t="n">
+      <c r="C18" s="23" t="n">
         <v>86.19</v>
       </c>
     </row>
@@ -917,10 +1151,10 @@
           <t>isForcedMilitary</t>
         </is>
       </c>
-      <c r="B19" s="13" t="n">
+      <c r="B19" s="24" t="n">
         <v>83914</v>
       </c>
-      <c r="C19" t="n">
+      <c r="C19" s="25" t="n">
         <v>85.84999999999999</v>
       </c>
     </row>
@@ -930,10 +1164,10 @@
           <t>isOrganRemoval</t>
         </is>
       </c>
-      <c r="B20" s="13" t="n">
+      <c r="B20" s="24" t="n">
         <v>83914</v>
       </c>
-      <c r="C20" t="n">
+      <c r="C20" s="25" t="n">
         <v>85.84999999999999</v>
       </c>
     </row>
@@ -943,10 +1177,10 @@
           <t>meansOfControlRestrictsMovement</t>
         </is>
       </c>
-      <c r="B21" s="13" t="n">
+      <c r="B21" s="24" t="n">
         <v>83637</v>
       </c>
-      <c r="C21" t="n">
+      <c r="C21" s="25" t="n">
         <v>85.56</v>
       </c>
     </row>
@@ -956,10 +1190,10 @@
           <t>meansOfControlPsychologicalAbuse</t>
         </is>
       </c>
-      <c r="B22" s="14" t="n">
+      <c r="B22" s="26" t="n">
         <v>83014</v>
       </c>
-      <c r="C22" t="n">
+      <c r="C22" s="27" t="n">
         <v>84.92</v>
       </c>
     </row>
@@ -969,10 +1203,10 @@
           <t>meansOfControlThreats</t>
         </is>
       </c>
-      <c r="B23" s="15" t="n">
+      <c r="B23" s="28" t="n">
         <v>82223</v>
       </c>
-      <c r="C23" t="n">
+      <c r="C23" s="29" t="n">
         <v>84.12</v>
       </c>
     </row>
@@ -982,10 +1216,10 @@
           <t>typeOfSexConcatenated</t>
         </is>
       </c>
-      <c r="B24" s="16" t="n">
+      <c r="B24" s="30" t="n">
         <v>81992</v>
       </c>
-      <c r="C24" t="n">
+      <c r="C24" s="31" t="n">
         <v>83.88</v>
       </c>
     </row>
@@ -995,10 +1229,10 @@
           <t>typeOfLabourConcatenated</t>
         </is>
       </c>
-      <c r="B25" s="17" t="n">
+      <c r="B25" s="32" t="n">
         <v>81137</v>
       </c>
-      <c r="C25" t="n">
+      <c r="C25" s="33" t="n">
         <v>83</v>
       </c>
     </row>
@@ -1008,10 +1242,10 @@
           <t>majorityStatusAtExploit</t>
         </is>
       </c>
-      <c r="B26" s="18" t="n">
+      <c r="B26" s="34" t="n">
         <v>76464</v>
       </c>
-      <c r="C26" t="n">
+      <c r="C26" s="35" t="n">
         <v>78.22</v>
       </c>
     </row>
@@ -1021,10 +1255,10 @@
           <t>typeOfSexPrivateSexualServices</t>
         </is>
       </c>
-      <c r="B27" s="19" t="n">
+      <c r="B27" s="36" t="n">
         <v>68583</v>
       </c>
-      <c r="C27" t="n">
+      <c r="C27" s="37" t="n">
         <v>70.16</v>
       </c>
     </row>
@@ -1034,10 +1268,10 @@
           <t>isAbduction</t>
         </is>
       </c>
-      <c r="B28" s="20" t="n">
+      <c r="B28" s="38" t="n">
         <v>67328</v>
       </c>
-      <c r="C28" t="n">
+      <c r="C28" s="39" t="n">
         <v>68.88</v>
       </c>
     </row>
@@ -1047,10 +1281,10 @@
           <t>typeOfSexRemoteInteractiveServices</t>
         </is>
       </c>
-      <c r="B29" s="21" t="n">
+      <c r="B29" s="40" t="n">
         <v>67018</v>
       </c>
-      <c r="C29" t="n">
+      <c r="C29" s="41" t="n">
         <v>68.56</v>
       </c>
     </row>
@@ -1060,10 +1294,10 @@
           <t>typeOfSexPornography</t>
         </is>
       </c>
-      <c r="B30" s="21" t="n">
+      <c r="B30" s="40" t="n">
         <v>67018</v>
       </c>
-      <c r="C30" t="n">
+      <c r="C30" s="41" t="n">
         <v>68.56</v>
       </c>
     </row>
@@ -1073,10 +1307,10 @@
           <t>typeOfSexProstitution</t>
         </is>
       </c>
-      <c r="B31" s="22" t="n">
+      <c r="B31" s="42" t="n">
         <v>58088</v>
       </c>
-      <c r="C31" t="n">
+      <c r="C31" s="43" t="n">
         <v>59.43</v>
       </c>
     </row>
@@ -1086,10 +1320,10 @@
           <t>ageBroad</t>
         </is>
       </c>
-      <c r="B32" s="23" t="n">
+      <c r="B32" s="44" t="n">
         <v>46783</v>
       </c>
-      <c r="C32" t="n">
+      <c r="C32" s="45" t="n">
         <v>47.86</v>
       </c>
     </row>
@@ -1099,10 +1333,10 @@
           <t>citizenship</t>
         </is>
       </c>
-      <c r="B33" s="24" t="n">
+      <c r="B33" s="46" t="n">
         <v>44460</v>
       </c>
-      <c r="C33" t="n">
+      <c r="C33" s="47" t="n">
         <v>45.48</v>
       </c>
     </row>
@@ -1112,10 +1346,10 @@
           <t>recruiterRelationFriend</t>
         </is>
       </c>
-      <c r="B34" s="25" t="n">
+      <c r="B34" s="48" t="n">
         <v>39787</v>
       </c>
-      <c r="C34" t="n">
+      <c r="C34" s="49" t="n">
         <v>40.7</v>
       </c>
     </row>
@@ -1125,10 +1359,10 @@
           <t>recruiterRelationIntimatePartner</t>
         </is>
       </c>
-      <c r="B35" s="25" t="n">
+      <c r="B35" s="48" t="n">
         <v>39787</v>
       </c>
-      <c r="C35" t="n">
+      <c r="C35" s="49" t="n">
         <v>40.7</v>
       </c>
     </row>
@@ -1138,10 +1372,10 @@
           <t>recruiterRelationOther</t>
         </is>
       </c>
-      <c r="B36" s="25" t="n">
+      <c r="B36" s="48" t="n">
         <v>39787</v>
       </c>
-      <c r="C36" t="n">
+      <c r="C36" s="49" t="n">
         <v>40.7</v>
       </c>
     </row>
@@ -1151,10 +1385,10 @@
           <t>recruiterRelationFamily</t>
         </is>
       </c>
-      <c r="B37" s="25" t="n">
+      <c r="B37" s="48" t="n">
         <v>39787</v>
       </c>
-      <c r="C37" t="n">
+      <c r="C37" s="49" t="n">
         <v>40.7</v>
       </c>
     </row>
@@ -1164,10 +1398,10 @@
           <t>meansOfControlConcatenated</t>
         </is>
       </c>
-      <c r="B38" s="26" t="n">
+      <c r="B38" s="50" t="n">
         <v>39435</v>
       </c>
-      <c r="C38" t="n">
+      <c r="C38" s="51" t="n">
         <v>40.34</v>
       </c>
     </row>
@@ -1177,10 +1411,10 @@
           <t>RecruiterRelationship</t>
         </is>
       </c>
-      <c r="B39" s="27" t="n">
+      <c r="B39" s="52" t="n">
         <v>38565</v>
       </c>
-      <c r="C39" t="n">
+      <c r="C39" s="53" t="n">
         <v>39.45</v>
       </c>
     </row>
@@ -1190,10 +1424,10 @@
           <t>typeOfLabourIllicitActivities</t>
         </is>
       </c>
-      <c r="B40" s="28" t="n">
+      <c r="B40" s="54" t="n">
         <v>36264</v>
       </c>
-      <c r="C40" t="n">
+      <c r="C40" s="55" t="n">
         <v>37.1</v>
       </c>
     </row>
@@ -1203,10 +1437,10 @@
           <t>typeOfLabourPeddling</t>
         </is>
       </c>
-      <c r="B41" s="28" t="n">
+      <c r="B41" s="54" t="n">
         <v>36264</v>
       </c>
-      <c r="C41" t="n">
+      <c r="C41" s="55" t="n">
         <v>37.1</v>
       </c>
     </row>
@@ -1216,10 +1450,10 @@
           <t>typeOfLabourMiningOrDrilling</t>
         </is>
       </c>
-      <c r="B42" s="28" t="n">
+      <c r="B42" s="54" t="n">
         <v>36186</v>
       </c>
-      <c r="C42" t="n">
+      <c r="C42" s="55" t="n">
         <v>37.02</v>
       </c>
     </row>
@@ -1229,10 +1463,10 @@
           <t>typeOfLabourBegging</t>
         </is>
       </c>
-      <c r="B43" s="28" t="n">
+      <c r="B43" s="54" t="n">
         <v>36186</v>
       </c>
-      <c r="C43" t="n">
+      <c r="C43" s="55" t="n">
         <v>37.02</v>
       </c>
     </row>
@@ -1242,10 +1476,10 @@
           <t>typeOfLabourTransportation</t>
         </is>
       </c>
-      <c r="B44" s="28" t="n">
+      <c r="B44" s="54" t="n">
         <v>36186</v>
       </c>
-      <c r="C44" t="n">
+      <c r="C44" s="55" t="n">
         <v>37.02</v>
       </c>
     </row>
@@ -1255,10 +1489,10 @@
           <t>typeOfLabourAquafarming</t>
         </is>
       </c>
-      <c r="B45" s="28" t="n">
+      <c r="B45" s="54" t="n">
         <v>36173</v>
       </c>
-      <c r="C45" t="n">
+      <c r="C45" s="55" t="n">
         <v>37.01</v>
       </c>
     </row>
@@ -1268,10 +1502,10 @@
           <t>typeOfLabourAgriculture</t>
         </is>
       </c>
-      <c r="B46" s="28" t="n">
+      <c r="B46" s="54" t="n">
         <v>36144</v>
       </c>
-      <c r="C46" t="n">
+      <c r="C46" s="55" t="n">
         <v>36.98</v>
       </c>
     </row>
@@ -1281,10 +1515,10 @@
           <t>typeOfLabourManufacturing</t>
         </is>
       </c>
-      <c r="B47" s="28" t="n">
+      <c r="B47" s="54" t="n">
         <v>36074</v>
       </c>
-      <c r="C47" t="n">
+      <c r="C47" s="55" t="n">
         <v>36.9</v>
       </c>
     </row>
@@ -1294,10 +1528,10 @@
           <t>typeOfLabourConstruction</t>
         </is>
       </c>
-      <c r="B48" s="29" t="n">
+      <c r="B48" s="56" t="n">
         <v>35864</v>
       </c>
-      <c r="C48" t="n">
+      <c r="C48" s="57" t="n">
         <v>36.69</v>
       </c>
     </row>
@@ -1307,10 +1541,10 @@
           <t>isSexAndLabour</t>
         </is>
       </c>
-      <c r="B49" s="30" t="n">
+      <c r="B49" s="58" t="n">
         <v>35182</v>
       </c>
-      <c r="C49" t="n">
+      <c r="C49" s="59" t="n">
         <v>35.99</v>
       </c>
     </row>
@@ -1320,10 +1554,10 @@
           <t>typeOfLabourHospitality</t>
         </is>
       </c>
-      <c r="B50" s="30" t="n">
+      <c r="B50" s="58" t="n">
         <v>35032</v>
       </c>
-      <c r="C50" t="n">
+      <c r="C50" s="59" t="n">
         <v>35.84</v>
       </c>
     </row>
@@ -1333,10 +1567,10 @@
           <t>typeOfLabourOther</t>
         </is>
       </c>
-      <c r="B51" s="30" t="n">
+      <c r="B51" s="58" t="n">
         <v>35025</v>
       </c>
-      <c r="C51" t="n">
+      <c r="C51" s="59" t="n">
         <v>35.83</v>
       </c>
     </row>
@@ -1346,10 +1580,10 @@
           <t>typeOfLabourNotSpecified</t>
         </is>
       </c>
-      <c r="B52" s="31" t="n">
+      <c r="B52" s="60" t="n">
         <v>34534</v>
       </c>
-      <c r="C52" t="n">
+      <c r="C52" s="61" t="n">
         <v>35.33</v>
       </c>
     </row>
@@ -1359,10 +1593,10 @@
           <t>typeOfLabourDomesticWork</t>
         </is>
       </c>
-      <c r="B53" s="32" t="n">
+      <c r="B53" s="62" t="n">
         <v>34055</v>
       </c>
-      <c r="C53" t="n">
+      <c r="C53" s="63" t="n">
         <v>34.84</v>
       </c>
     </row>
@@ -1372,10 +1606,10 @@
           <t>isSexualExploit</t>
         </is>
       </c>
-      <c r="B54" s="33" t="n">
+      <c r="B54" s="64" t="n">
         <v>32349</v>
       </c>
-      <c r="C54" t="n">
+      <c r="C54" s="65" t="n">
         <v>33.09</v>
       </c>
     </row>
@@ -1385,10 +1619,10 @@
           <t>isForcedLabour</t>
         </is>
       </c>
-      <c r="B55" s="33" t="n">
+      <c r="B55" s="64" t="n">
         <v>32103</v>
       </c>
-      <c r="C55" t="n">
+      <c r="C55" s="65" t="n">
         <v>32.84</v>
       </c>
     </row>
@@ -1398,10 +1632,10 @@
           <t>typeOfExploitConcatenated</t>
         </is>
       </c>
-      <c r="B56" s="34" t="n">
+      <c r="B56" s="66" t="n">
         <v>31461</v>
       </c>
-      <c r="C56" t="n">
+      <c r="C56" s="67" t="n">
         <v>32.19</v>
       </c>
     </row>
@@ -1411,10 +1645,10 @@
           <t>majorityStatus</t>
         </is>
       </c>
-      <c r="B57" s="35" t="n">
+      <c r="B57" s="68" t="n">
         <v>26504</v>
       </c>
-      <c r="C57" t="n">
+      <c r="C57" s="69" t="n">
         <v>27.11</v>
       </c>
     </row>
@@ -1424,10 +1658,10 @@
           <t>isOtherExploit</t>
         </is>
       </c>
-      <c r="B58" s="36" t="n">
+      <c r="B58" s="70" t="n">
         <v>24329</v>
       </c>
-      <c r="C58" t="n">
+      <c r="C58" s="71" t="n">
         <v>24.89</v>
       </c>
     </row>
@@ -1437,10 +1671,10 @@
           <t>CountryOfExploitation</t>
         </is>
       </c>
-      <c r="B59" s="36" t="n">
+      <c r="B59" s="70" t="n">
         <v>24258</v>
       </c>
-      <c r="C59" t="n">
+      <c r="C59" s="71" t="n">
         <v>24.82</v>
       </c>
     </row>
@@ -1450,10 +1684,10 @@
           <t>meansOfControlNotSpecified</t>
         </is>
       </c>
-      <c r="B60" s="37" t="n">
+      <c r="B60" s="72" t="n">
         <v>13967</v>
       </c>
-      <c r="C60" t="n">
+      <c r="C60" s="73" t="n">
         <v>14.29</v>
       </c>
     </row>
@@ -1463,10 +1697,10 @@
           <t>gender</t>
         </is>
       </c>
-      <c r="B61" s="38" t="n">
+      <c r="B61" s="74" t="n">
         <v>8138</v>
       </c>
-      <c r="C61" t="n">
+      <c r="C61" s="75" t="n">
         <v>8.33</v>
       </c>
     </row>
@@ -1476,10 +1710,10 @@
           <t>yearOfRegistration</t>
         </is>
       </c>
-      <c r="B62" s="39" t="n">
+      <c r="B62" s="76" t="n">
         <v>2011</v>
       </c>
-      <c r="C62" t="n">
+      <c r="C62" s="77" t="n">
         <v>2.06</v>
       </c>
     </row>
@@ -1489,10 +1723,10 @@
           <t>recruiterRelationUnknown</t>
         </is>
       </c>
-      <c r="B63" s="40" t="n">
+      <c r="B63" s="78" t="n">
         <v>236</v>
       </c>
-      <c r="C63" t="n">
+      <c r="C63" s="79" t="n">
         <v>0.24</v>
       </c>
     </row>

</xml_diff>